<commit_message>
Upgrade training table display
</commit_message>
<xml_diff>
--- a/data/training_videos.xlsx
+++ b/data/training_videos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82249B3-BBC7-BD43-8109-A2B0AB9329B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DAC0E8-7634-E64F-9045-C16824FA38E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,11 +23,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet6!$A$2:$C$92</definedName>
   </definedNames>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="23" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="425">
   <si>
     <t xml:space="preserve"> Arrangements  </t>
   </si>
@@ -458,15 +469,9 @@
     <t>Show File Handling</t>
   </si>
   <si>
-    <t>Core skill. Saving and restoring show files is a good thing for all to know.</t>
-  </si>
-  <si>
     <t>Record to Playback Sequence</t>
   </si>
   <si>
-    <t>We could occasionally use a Sequence to automate a complicated set of steps.</t>
-  </si>
-  <si>
     <t>Edit Cues and Sequences</t>
   </si>
   <si>
@@ -476,9 +481,6 @@
     <t>May not be relevant to current fixtures</t>
   </si>
   <si>
-    <t>Cues are useful when you want to completely change the look quickly and you can plan ahead.</t>
-  </si>
-  <si>
     <t>Patching - Add Dimmer</t>
   </si>
   <si>
@@ -962,9 +964,6 @@
     <t>Volunteer Operator's Guide To ProPresenter 7</t>
   </si>
   <si>
-    <t>33:21</t>
-  </si>
-  <si>
     <t>1:13:38</t>
   </si>
   <si>
@@ -989,51 +988,30 @@
     <t>Not relevant to UAC</t>
   </si>
   <si>
-    <t>7:40</t>
-  </si>
-  <si>
     <t>Screen Configuration</t>
   </si>
   <si>
-    <t>5:17</t>
-  </si>
-  <si>
     <t xml:space="preserve">Interface Overview </t>
   </si>
   <si>
     <t>Search</t>
   </si>
   <si>
-    <t>3:43</t>
-  </si>
-  <si>
     <t>The Announcements Layer</t>
   </si>
   <si>
-    <t>3:56</t>
-  </si>
-  <si>
     <t>Show Controls (Audio, Stage Controls, Timers, Messages, Props)</t>
   </si>
   <si>
-    <t>13:37</t>
-  </si>
-  <si>
     <t>How to use Timers &amp; Countdowns</t>
   </si>
   <si>
-    <t>10:24</t>
-  </si>
-  <si>
     <t>ProPresenter7</t>
   </si>
   <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219261</t>
   </si>
   <si>
-    <t>6:11</t>
-  </si>
-  <si>
     <t>Using the Presentation Editor</t>
   </si>
   <si>
@@ -1043,15 +1021,9 @@
     <t>Stage Screens</t>
   </si>
   <si>
-    <t>5:06</t>
-  </si>
-  <si>
     <t>Looks</t>
   </si>
   <si>
-    <t>5:41</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219263</t>
   </si>
   <si>
@@ -1061,42 +1033,27 @@
     <t>Using Bibles</t>
   </si>
   <si>
-    <t>3:42</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219265</t>
   </si>
   <si>
     <t>Working with Audio</t>
   </si>
   <si>
-    <t>3:44</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219247</t>
   </si>
   <si>
     <t>How to use Macros</t>
   </si>
   <si>
-    <t>12:55</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219267</t>
   </si>
   <si>
     <t>Easyview</t>
   </si>
   <si>
-    <t>1:41</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219274</t>
   </si>
   <si>
-    <t>10:59</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219275</t>
   </si>
   <si>
@@ -1106,24 +1063,15 @@
     <t>ATEM + ProPresenter</t>
   </si>
   <si>
-    <t>19:51</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#219278</t>
   </si>
   <si>
-    <t>7:19</t>
-  </si>
-  <si>
     <t>Operator View</t>
   </si>
   <si>
     <t>Working with text across multiple screens</t>
   </si>
   <si>
-    <t>9:33</t>
-  </si>
-  <si>
     <t>https://renewedvision.com/propresenter/tutorials/#220536</t>
   </si>
   <si>
@@ -1134,6 +1082,246 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>0:22:05</t>
+  </si>
+  <si>
+    <t>0:7:31</t>
+  </si>
+  <si>
+    <t>0:10:55</t>
+  </si>
+  <si>
+    <t>0:3:34</t>
+  </si>
+  <si>
+    <t>0:7:05</t>
+  </si>
+  <si>
+    <t>0:9:10</t>
+  </si>
+  <si>
+    <t>0:5:27</t>
+  </si>
+  <si>
+    <t>0:9:37</t>
+  </si>
+  <si>
+    <t>0:0:51</t>
+  </si>
+  <si>
+    <t>0:8:32</t>
+  </si>
+  <si>
+    <t>0:7:28</t>
+  </si>
+  <si>
+    <t>0:5:09</t>
+  </si>
+  <si>
+    <t>0:2:27</t>
+  </si>
+  <si>
+    <t>0:7:23</t>
+  </si>
+  <si>
+    <t>0:6:54</t>
+  </si>
+  <si>
+    <t>0:7:29</t>
+  </si>
+  <si>
+    <t>0:12:38</t>
+  </si>
+  <si>
+    <t>0:33:21</t>
+  </si>
+  <si>
+    <t>0:7:40</t>
+  </si>
+  <si>
+    <t>0:3:43</t>
+  </si>
+  <si>
+    <t>0:13:37</t>
+  </si>
+  <si>
+    <t>0:6:11</t>
+  </si>
+  <si>
+    <t>0:3:42</t>
+  </si>
+  <si>
+    <t>0:1:41</t>
+  </si>
+  <si>
+    <t>0:10:24</t>
+  </si>
+  <si>
+    <t>0:5:06</t>
+  </si>
+  <si>
+    <t>0:5:41</t>
+  </si>
+  <si>
+    <t>0:3:44</t>
+  </si>
+  <si>
+    <t>0:12:55</t>
+  </si>
+  <si>
+    <t>0:9:33</t>
+  </si>
+  <si>
+    <t>0:5:17</t>
+  </si>
+  <si>
+    <t>0:3:56</t>
+  </si>
+  <si>
+    <t>0:10:59</t>
+  </si>
+  <si>
+    <t>0:19:51</t>
+  </si>
+  <si>
+    <t>0:7:19</t>
+  </si>
+  <si>
+    <t>0:07:01</t>
+  </si>
+  <si>
+    <t>0:02:38</t>
+  </si>
+  <si>
+    <t>0:03:36</t>
+  </si>
+  <si>
+    <t>0:08:40</t>
+  </si>
+  <si>
+    <t>0:08:00</t>
+  </si>
+  <si>
+    <t>0:10:31</t>
+  </si>
+  <si>
+    <t>0:09:38</t>
+  </si>
+  <si>
+    <t>0:06:08</t>
+  </si>
+  <si>
+    <t>0:06:00</t>
+  </si>
+  <si>
+    <t>0:10:33</t>
+  </si>
+  <si>
+    <t>0:05:41</t>
+  </si>
+  <si>
+    <t>0:04:40</t>
+  </si>
+  <si>
+    <t>0:09:14</t>
+  </si>
+  <si>
+    <t>0:04:13</t>
+  </si>
+  <si>
+    <t>0:01:48</t>
+  </si>
+  <si>
+    <t>0:09:48</t>
+  </si>
+  <si>
+    <t>0:07:18</t>
+  </si>
+  <si>
+    <t>0:06:52</t>
+  </si>
+  <si>
+    <t>0:05:47</t>
+  </si>
+  <si>
+    <t>0:07:36</t>
+  </si>
+  <si>
+    <t>0:06:22</t>
+  </si>
+  <si>
+    <t>0:07:02</t>
+  </si>
+  <si>
+    <t>0:06:26</t>
+  </si>
+  <si>
+    <t>0:03:39</t>
+  </si>
+  <si>
+    <t>0:03:02</t>
+  </si>
+  <si>
+    <t>0:02:21</t>
+  </si>
+  <si>
+    <t>0:05:14</t>
+  </si>
+  <si>
+    <t>0:03:06</t>
+  </si>
+  <si>
+    <t>0:03:40</t>
+  </si>
+  <si>
+    <t>0:04:53</t>
+  </si>
+  <si>
+    <t>0:04:00</t>
+  </si>
+  <si>
+    <t>0:03:37</t>
+  </si>
+  <si>
+    <t>0:02:03</t>
+  </si>
+  <si>
+    <t>0:03:38</t>
+  </si>
+  <si>
+    <t>0:03:01</t>
+  </si>
+  <si>
+    <t>0:04:25</t>
+  </si>
+  <si>
+    <t>0:05:19</t>
+  </si>
+  <si>
+    <t>0:01:49</t>
+  </si>
+  <si>
+    <t>0:02:24</t>
+  </si>
+  <si>
+    <t>0:02:48</t>
+  </si>
+  <si>
+    <t>0:02:51</t>
+  </si>
+  <si>
+    <t>0:03:29</t>
+  </si>
+  <si>
+    <t>Saving and restoring show files is a good for all to know.</t>
+  </si>
+  <si>
+    <t>Useful when you want to change the look quickly and you can plan ahead.</t>
+  </si>
+  <si>
+    <t>We could use a Sequence to automate a complicated set of steps.</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1431,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="11"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1266,7 +1454,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1277,9 +1464,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1288,6 +1472,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1583,7 +1776,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1640,7 +1833,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1697,7 +1890,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1754,7 +1947,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1811,7 +2004,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3101,7 +3294,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisCol" showAll="0">
@@ -3212,12 +3405,7 @@
   <autoFilter ref="A1:J116" xr:uid="{486948C8-A13F-A545-90E9-87DFED66A023}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Projection"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="ProPresenter"/>
+        <filter val="Lighting"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3584,15 +3772,15 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>84</v>
@@ -3607,20 +3795,20 @@
         <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -3643,7 +3831,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3662,7 +3850,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -3685,7 +3873,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -3702,12 +3890,12 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B12">
         <v>22</v>
@@ -3742,8 +3930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G100" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3753,7 +3941,7 @@
     <col min="3" max="3" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="41" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="17" customWidth="1"/>
     <col min="7" max="7" width="73.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
@@ -3771,25 +3959,25 @@
         <v>107</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>229</v>
+      <c r="F1" s="17" t="s">
+        <v>226</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>103</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3813,7 +4001,7 @@
         <v>111</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3837,7 +4025,7 @@
         <v>111</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3861,7 +4049,7 @@
         <v>111</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3885,7 +4073,7 @@
         <v>111</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3909,7 +4097,7 @@
         <v>111</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3933,7 +4121,7 @@
         <v>111</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -3971,19 +4159,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0.29236111111111113</v>
+        <v>227</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>380</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4000,19 +4188,19 @@
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="F10" s="12">
-        <v>0.10972222222222222</v>
+        <v>231</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>381</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4029,19 +4217,19 @@
         <v>3</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F11" s="12">
-        <v>0.15</v>
+        <v>230</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>382</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4058,19 +4246,19 @@
         <v>4</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0.3611111111111111</v>
+        <v>252</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>383</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4087,19 +4275,19 @@
         <v>5</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0.33333333333333331</v>
+        <v>262</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>384</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4116,19 +4304,19 @@
         <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0.4381944444444445</v>
+        <v>266</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>385</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4142,16 +4330,16 @@
         <v>114</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F15" s="12">
-        <v>0.40138888888888885</v>
+        <v>253</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>386</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4165,16 +4353,16 @@
         <v>114</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0.25555555555555559</v>
+        <v>254</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>387</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4188,19 +4376,19 @@
         <v>114</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F17" s="12">
-        <v>0.25</v>
+        <v>256</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>388</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4214,16 +4402,16 @@
         <v>114</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F18" s="12">
-        <v>0.43958333333333338</v>
+        <v>258</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>389</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4237,16 +4425,16 @@
         <v>114</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.23680555555555557</v>
+        <v>257</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>390</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4260,16 +4448,16 @@
         <v>114</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0.19444444444444445</v>
+        <v>259</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>391</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4283,13 +4471,13 @@
         <v>114</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F21" s="12">
-        <v>0.38472222222222219</v>
+        <v>261</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>392</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -4305,13 +4493,13 @@
         <v>114</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F22" s="12">
-        <v>0.17569444444444446</v>
+        <v>264</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>393</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -4327,13 +4515,13 @@
         <v>114</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F23" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>264</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>394</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -4349,13 +4537,13 @@
         <v>114</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="F24" s="12">
-        <v>0.40277777777777773</v>
+        <v>268</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>395</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -4371,13 +4559,13 @@
         <v>114</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="F25" s="12">
-        <v>0.30416666666666664</v>
+        <v>270</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>396</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -4393,10 +4581,10 @@
         <v>114</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F26" s="12">
-        <v>0.28611111111111115</v>
+        <v>264</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>397</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -4419,7 +4607,7 @@
         <v>89</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4440,7 +4628,7 @@
         <v>91</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -4461,10 +4649,10 @@
         <v>88</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>72</v>
       </c>
@@ -4485,10 +4673,10 @@
         <v>111</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>72</v>
       </c>
@@ -4509,10 +4697,10 @@
         <v>111</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>72</v>
       </c>
@@ -4525,23 +4713,23 @@
       <c r="D32" s="3">
         <v>1</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="F32" s="15">
-        <v>3.65</v>
+      <c r="F32" s="24" t="s">
+        <v>403</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>72</v>
       </c>
@@ -4554,23 +4742,23 @@
       <c r="D33" s="3">
         <v>2</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F33" s="15">
-        <v>3.02</v>
+      <c r="F33" s="24" t="s">
+        <v>404</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>72</v>
       </c>
@@ -4583,23 +4771,24 @@
       <c r="D34" s="3">
         <v>3</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F34" s="15">
-        <v>2.35</v>
-      </c>
+      <c r="F34" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="G34" s="25"/>
       <c r="H34" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>72</v>
       </c>
@@ -4612,23 +4801,23 @@
       <c r="D35" s="3">
         <v>4</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="F35" s="15">
-        <v>5.23</v>
+      <c r="F35" s="24" t="s">
+        <v>406</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>72</v>
       </c>
@@ -4636,28 +4825,28 @@
         <v>96</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>161</v>
+        <v>299</v>
       </c>
       <c r="D36" s="3">
         <v>3</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="F36" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="G36" s="15" t="s">
+      <c r="F36" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="G36" s="14" t="s">
         <v>138</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
@@ -4670,26 +4859,26 @@
       <c r="D37" s="3">
         <v>5</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="F37" s="15">
-        <v>3.67</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>140</v>
+      <c r="F37" s="24" t="s">
+        <v>408</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>422</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>72</v>
       </c>
@@ -4697,31 +4886,31 @@
         <v>96</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="F38" s="15">
-        <v>4.88</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>146</v>
+      <c r="E38" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>423</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -4729,31 +4918,31 @@
         <v>96</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D39" s="3">
         <v>2</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F39" s="15">
-        <v>4</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>146</v>
+      <c r="E39" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>423</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>72</v>
       </c>
@@ -4761,31 +4950,31 @@
         <v>96</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D40" s="3">
         <v>3</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" s="15">
-        <v>3.62</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>142</v>
+      <c r="E40" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>424</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>72</v>
       </c>
@@ -4793,28 +4982,28 @@
         <v>96</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D41" s="3">
         <v>1</v>
       </c>
-      <c r="E41" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="F41" s="15">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>148</v>
+      <c r="E41" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>72</v>
       </c>
@@ -4822,28 +5011,28 @@
         <v>96</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D42" s="3">
         <v>2</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F42" s="15">
-        <v>3.63</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>148</v>
+      <c r="E42" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>72</v>
       </c>
@@ -4851,28 +5040,28 @@
         <v>96</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D43" s="3">
         <v>4</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="F43" s="15">
-        <v>3.02</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>148</v>
+      <c r="E43" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>145</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>72</v>
       </c>
@@ -4880,28 +5069,28 @@
         <v>96</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D44" s="3">
         <v>5</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="F44" s="15">
-        <v>4.42</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>145</v>
+      <c r="E44" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>415</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>72</v>
       </c>
@@ -4909,28 +5098,28 @@
         <v>96</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D45" s="3">
         <v>6</v>
       </c>
-      <c r="E45" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="F45" s="15">
-        <v>5.32</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>153</v>
+      <c r="E45" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>72</v>
       </c>
@@ -4938,28 +5127,28 @@
         <v>96</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D46" s="3">
         <v>7</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="F46" s="15">
-        <v>1.82</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>153</v>
+      <c r="E46" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>417</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>72</v>
       </c>
@@ -4967,28 +5156,28 @@
         <v>96</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D47" s="3">
         <v>8</v>
       </c>
-      <c r="E47" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="F47" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>153</v>
+      <c r="E47" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>72</v>
       </c>
@@ -4996,28 +5185,28 @@
         <v>96</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D48" s="3">
         <v>9</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="F48" s="15">
-        <v>2.4</v>
-      </c>
-      <c r="G48" s="15" t="s">
+      <c r="E48" s="14" t="s">
         <v>153</v>
       </c>
+      <c r="F48" s="24" t="s">
+        <v>418</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>150</v>
+      </c>
       <c r="H48" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>72</v>
       </c>
@@ -5025,28 +5214,28 @@
         <v>96</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D49" s="3">
         <v>10</v>
       </c>
-      <c r="E49" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F49" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>153</v>
+      <c r="E49" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>419</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>72</v>
       </c>
@@ -5054,28 +5243,28 @@
         <v>96</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D50" s="3">
         <v>11</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="F50" s="15">
-        <v>2.85</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>162</v>
+      <c r="E50" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>159</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>72</v>
       </c>
@@ -5083,28 +5272,28 @@
         <v>96</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D51" s="3">
         <v>12</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="F51" s="15">
-        <v>3.48</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>160</v>
+      <c r="E51" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>157</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>72</v>
       </c>
@@ -5125,10 +5314,10 @@
         <v>130</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>72</v>
       </c>
@@ -5147,10 +5336,10 @@
         <v>129</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="19" hidden="1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>72</v>
       </c>
@@ -5163,23 +5352,23 @@
       <c r="D54" s="3">
         <v>1</v>
       </c>
-      <c r="E54" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="F54" s="17">
-        <v>0.24097222222222223</v>
+      <c r="E54" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="F54" s="23" t="s">
+        <v>398</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="19" hidden="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>72</v>
       </c>
@@ -5192,23 +5381,23 @@
       <c r="D55" s="3">
         <v>2</v>
       </c>
-      <c r="E55" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="F55" s="17">
-        <v>0.31666666666666665</v>
+      <c r="E55" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>399</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="19" hidden="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>72</v>
       </c>
@@ -5221,23 +5410,23 @@
       <c r="D56" s="3">
         <v>3</v>
       </c>
-      <c r="E56" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="F56" s="17">
-        <v>0.26527777777777778</v>
+      <c r="E56" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>400</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J56" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="3" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>72</v>
       </c>
@@ -5250,23 +5439,23 @@
       <c r="D57" s="3">
         <v>4</v>
       </c>
-      <c r="E57" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="F57" s="17">
-        <v>0.29305555555555557</v>
+      <c r="E57" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>401</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" s="3" customFormat="1" ht="19" hidden="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>72</v>
       </c>
@@ -5279,28 +5468,28 @@
       <c r="D58" s="3">
         <v>5</v>
       </c>
-      <c r="E58" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="F58" s="17">
-        <v>0.26805555555555555</v>
+      <c r="E58" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>402</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>122</v>
@@ -5313,12 +5502,12 @@
         <v>111</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>123</v>
@@ -5334,18 +5523,18 @@
       </c>
       <c r="F60" s="3"/>
       <c r="H60" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>123</v>
@@ -5357,107 +5546,107 @@
         <v>2</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F61" s="5"/>
       <c r="H61" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D62" s="3">
         <v>1</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3" t="s">
         <v>125</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D63" s="3">
         <v>2</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3" t="s">
         <v>126</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D64" s="3">
         <v>3</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3" t="s">
         <v>127</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -5481,7 +5670,7 @@
         <v>111</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -5505,7 +5694,7 @@
         <v>111</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -5529,7 +5718,7 @@
         <v>111</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -5553,7 +5742,7 @@
         <v>111</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -5577,15 +5766,15 @@
         <v>111</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>108</v>
@@ -5596,25 +5785,25 @@
       <c r="E70" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="19">
-        <v>0.92013888888888884</v>
+      <c r="F70" s="21" t="s">
+        <v>345</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>108</v>
@@ -5625,25 +5814,25 @@
       <c r="E71" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F71" s="19">
-        <v>0.31319444444444444</v>
+      <c r="F71" s="21" t="s">
+        <v>346</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>108</v>
@@ -5654,28 +5843,28 @@
       <c r="E72" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F72" s="19">
-        <v>0.4548611111111111</v>
+      <c r="F72" s="21" t="s">
+        <v>347</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>108</v>
@@ -5686,28 +5875,28 @@
       <c r="E73" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F73" s="19">
-        <v>0.14861111111111111</v>
+      <c r="F73" s="21" t="s">
+        <v>348</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>108</v>
@@ -5718,25 +5907,25 @@
       <c r="E74" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F74" s="19">
-        <v>0.2951388888888889</v>
+      <c r="F74" s="21" t="s">
+        <v>349</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>108</v>
@@ -5747,25 +5936,25 @@
       <c r="E75" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F75" s="19">
-        <v>0.38194444444444442</v>
+      <c r="F75" s="21" t="s">
+        <v>350</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>108</v>
@@ -5776,28 +5965,28 @@
       <c r="E76" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F76" s="19">
-        <v>0.22708333333333333</v>
+      <c r="F76" s="21" t="s">
+        <v>351</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>108</v>
@@ -5808,25 +5997,25 @@
       <c r="E77" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F77" s="19">
-        <v>0.40069444444444446</v>
+      <c r="F77" s="21" t="s">
+        <v>352</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I77" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>108</v>
@@ -5837,28 +6026,28 @@
       <c r="E78" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F78" s="19">
-        <v>3.5416666666666666E-2</v>
+      <c r="F78" s="21" t="s">
+        <v>353</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>108</v>
@@ -5869,25 +6058,25 @@
       <c r="E79" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F79" s="19">
-        <v>0.35555555555555557</v>
+      <c r="F79" s="21" t="s">
+        <v>354</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>109</v>
@@ -5898,25 +6087,25 @@
       <c r="E80" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F80" s="19">
-        <v>0.31111111111111112</v>
+      <c r="F80" s="21" t="s">
+        <v>355</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>109</v>
@@ -5925,27 +6114,27 @@
         <v>3</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="F81" s="19">
-        <v>0.21458333333333335</v>
+        <v>200</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>356</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I81" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>109</v>
@@ -5956,25 +6145,25 @@
       <c r="E82" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F82" s="19">
-        <v>0.10208333333333335</v>
+      <c r="F82" s="21" t="s">
+        <v>357</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>109</v>
@@ -5985,25 +6174,25 @@
       <c r="E83" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F83" s="19">
-        <v>0.30763888888888891</v>
+      <c r="F83" s="21" t="s">
+        <v>358</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>109</v>
@@ -6014,25 +6203,25 @@
       <c r="E84" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F84" s="19">
-        <v>0.28750000000000003</v>
+      <c r="F84" s="21" t="s">
+        <v>359</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>109</v>
@@ -6043,25 +6232,25 @@
       <c r="E85" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F85" s="19">
-        <v>0.31180555555555556</v>
+      <c r="F85" s="21" t="s">
+        <v>360</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I85" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>109</v>
@@ -6072,17 +6261,17 @@
       <c r="E86" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F86" s="19">
-        <v>0.52638888888888891</v>
+      <c r="F86" s="21" t="s">
+        <v>361</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I86" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -6106,7 +6295,7 @@
         <v>111</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J87" s="3"/>
     </row>
@@ -6131,7 +6320,7 @@
         <v>111</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J88" s="3"/>
     </row>
@@ -6156,7 +6345,7 @@
         <v>111</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J89" s="3"/>
     </row>
@@ -6172,13 +6361,13 @@
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>100</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J90" s="3"/>
     </row>
@@ -6197,7 +6386,7 @@
         <v>101</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J91" s="3"/>
     </row>
@@ -6217,7 +6406,7 @@
         <v>102</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J92" s="3"/>
     </row>
@@ -6247,7 +6436,7 @@
         <v>79</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>108</v>
@@ -6256,20 +6445,20 @@
         <v>1</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -6277,7 +6466,7 @@
         <v>79</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>108</v>
@@ -6286,20 +6475,20 @@
         <v>2</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -6318,12 +6507,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>108</v>
@@ -6332,25 +6521,25 @@
         <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F97" s="20" t="s">
-        <v>309</v>
+        <v>301</v>
+      </c>
+      <c r="F97" s="18" t="s">
+        <v>305</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I97" s="3"/>
       <c r="J97" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>108</v>
@@ -6359,25 +6548,25 @@
         <v>1</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="F98" s="21" t="s">
-        <v>308</v>
+        <v>304</v>
+      </c>
+      <c r="F98" s="19" t="s">
+        <v>362</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I98" s="3"/>
       <c r="J98" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>108</v>
@@ -6386,23 +6575,23 @@
         <v>2</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="F99" s="22" t="s">
-        <v>317</v>
+        <v>314</v>
+      </c>
+      <c r="F99" s="20" t="s">
+        <v>363</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>108</v>
@@ -6411,23 +6600,23 @@
         <v>3</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F100" s="22" t="s">
-        <v>322</v>
+        <v>315</v>
+      </c>
+      <c r="F100" s="20" t="s">
+        <v>364</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>108</v>
@@ -6436,23 +6625,23 @@
         <v>7</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="F101" s="22" t="s">
-        <v>326</v>
+        <v>317</v>
+      </c>
+      <c r="F101" s="20" t="s">
+        <v>365</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>108</v>
@@ -6461,23 +6650,23 @@
         <v>4</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="F102" s="22" t="s">
-        <v>331</v>
+        <v>321</v>
+      </c>
+      <c r="F102" s="20" t="s">
+        <v>366</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>108</v>
@@ -6486,23 +6675,23 @@
         <v>5</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="F103" s="22" t="s">
-        <v>341</v>
+        <v>327</v>
+      </c>
+      <c r="F103" s="20" t="s">
+        <v>367</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>108</v>
@@ -6511,23 +6700,23 @@
         <v>6</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F104" s="22" t="s">
-        <v>350</v>
+        <v>333</v>
+      </c>
+      <c r="F104" s="20" t="s">
+        <v>368</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>109</v>
@@ -6536,23 +6725,23 @@
         <v>6</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="F105" s="22" t="s">
-        <v>328</v>
+        <v>318</v>
+      </c>
+      <c r="F105" s="20" t="s">
+        <v>369</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>109</v>
@@ -6561,23 +6750,23 @@
         <v>1</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F106" s="22" t="s">
-        <v>335</v>
+        <v>323</v>
+      </c>
+      <c r="F106" s="20" t="s">
+        <v>370</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>109</v>
@@ -6586,23 +6775,23 @@
         <v>2</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="F107" s="22" t="s">
-        <v>337</v>
+        <v>324</v>
+      </c>
+      <c r="F107" s="20" t="s">
+        <v>371</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>109</v>
@@ -6611,23 +6800,23 @@
         <v>3</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="F108" s="22" t="s">
-        <v>344</v>
+        <v>329</v>
+      </c>
+      <c r="F108" s="20" t="s">
+        <v>372</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>109</v>
@@ -6636,23 +6825,23 @@
         <v>4</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="F109" s="22" t="s">
-        <v>347</v>
+        <v>331</v>
+      </c>
+      <c r="F109" s="20" t="s">
+        <v>373</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>109</v>
@@ -6661,163 +6850,163 @@
         <v>5</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="F110" s="22" t="s">
-        <v>361</v>
+        <v>340</v>
+      </c>
+      <c r="F110" s="20" t="s">
+        <v>374</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D111" s="3">
         <v>1</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="F111" s="22" t="s">
-        <v>319</v>
+        <v>313</v>
+      </c>
+      <c r="F111" s="20" t="s">
+        <v>375</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D112" s="3">
         <v>6</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F112" s="22" t="s">
-        <v>324</v>
+        <v>316</v>
+      </c>
+      <c r="F112" s="20" t="s">
+        <v>376</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D113" s="3">
         <v>2</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="F113" s="22" t="s">
-        <v>352</v>
+        <v>336</v>
+      </c>
+      <c r="F113" s="20" t="s">
+        <v>377</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D114" s="3">
         <v>3</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="F114" s="22" t="s">
-        <v>356</v>
+        <v>337</v>
+      </c>
+      <c r="F114" s="20" t="s">
+        <v>378</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D115" s="3">
         <v>4</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F115" s="22" t="s">
-        <v>358</v>
+        <v>339</v>
+      </c>
+      <c r="F115" s="20" t="s">
+        <v>379</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D116" s="3">
         <v>5</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="F116" s="22" t="s">
-        <v>363</v>
+        <v>343</v>
+      </c>
+      <c r="F116" s="20" t="s">
+        <v>342</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -6856,20 +7045,15 @@
     <hyperlink ref="H85" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
     <hyperlink ref="H84" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
     <hyperlink ref="H62" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="F54" r:id="rId26" display="5:47NOW PLAYING" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="F55" r:id="rId27" display="7:36NOW PLAYING" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="F56" r:id="rId28" display="6:22NOW PLAYING" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="F57" r:id="rId29" display="7:02NOW PLAYING" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="F58" r:id="rId30" display="6:26NOW PLAYING" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="H56" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="H71" r:id="rId32" xr:uid="{045D822F-D7EC-0843-BF87-B5E903B9062F}"/>
-    <hyperlink ref="H100" r:id="rId33" location="219259" xr:uid="{AD0D256B-219F-2F46-BC7F-4D31F0C183BB}"/>
-    <hyperlink ref="H101" r:id="rId34" location="218515" xr:uid="{807693E7-BD7A-3F4E-8C5A-771DA977A842}"/>
+    <hyperlink ref="H56" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="H71" r:id="rId27" xr:uid="{045D822F-D7EC-0843-BF87-B5E903B9062F}"/>
+    <hyperlink ref="H100" r:id="rId28" location="219259" xr:uid="{AD0D256B-219F-2F46-BC7F-4D31F0C183BB}"/>
+    <hyperlink ref="H101" r:id="rId29" location="218515" xr:uid="{807693E7-BD7A-3F4E-8C5A-771DA977A842}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -7119,10 +7303,10 @@
       <c r="A2">
         <v>12</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="13">
         <v>0.40138888888888885</v>
       </c>
     </row>
@@ -7131,9 +7315,9 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="14">
+        <v>237</v>
+      </c>
+      <c r="C3" s="13">
         <v>0.38472222222222219</v>
       </c>
     </row>
@@ -7141,10 +7325,10 @@
       <c r="A4">
         <v>11</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="13">
         <v>0.3611111111111111</v>
       </c>
     </row>
@@ -7152,10 +7336,10 @@
       <c r="A5">
         <v>15</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="C5" s="14">
+      <c r="B5" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="13">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -7163,10 +7347,10 @@
       <c r="A6">
         <v>14</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="B6" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="13">
         <v>0.29305555555555557</v>
       </c>
     </row>
@@ -7174,10 +7358,10 @@
       <c r="A7">
         <v>16</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="B7" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="13">
         <v>0.25555555555555559</v>
       </c>
     </row>
@@ -7186,9 +7370,9 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C8" s="14">
+        <v>236</v>
+      </c>
+      <c r="C8" s="13">
         <v>0.25</v>
       </c>
     </row>
@@ -7196,10 +7380,10 @@
       <c r="A9">
         <v>13</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="B9" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="13">
         <v>0.23680555555555557</v>
       </c>
     </row>
@@ -7208,9 +7392,9 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C10" s="14">
+        <v>240</v>
+      </c>
+      <c r="C10" s="13">
         <v>0.19444444444444445</v>
       </c>
     </row>
@@ -7219,9 +7403,9 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>236</v>
-      </c>
-      <c r="C11" s="14">
+        <v>233</v>
+      </c>
+      <c r="C11" s="13">
         <v>0.17569444444444446</v>
       </c>
     </row>
@@ -7230,9 +7414,9 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
-      </c>
-      <c r="C12" s="14">
+        <v>241</v>
+      </c>
+      <c r="C12" s="13">
         <v>0.11041666666666666</v>
       </c>
     </row>
@@ -7241,9 +7425,9 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" s="14">
+        <v>239</v>
+      </c>
+      <c r="C13" s="13">
         <v>0.43958333333333338</v>
       </c>
     </row>
@@ -7252,9 +7436,9 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>245</v>
-      </c>
-      <c r="C14" s="14">
+        <v>242</v>
+      </c>
+      <c r="C14" s="13">
         <v>0.4381944444444445</v>
       </c>
     </row>
@@ -7263,9 +7447,9 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>241</v>
-      </c>
-      <c r="C15" s="14">
+        <v>238</v>
+      </c>
+      <c r="C15" s="13">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
@@ -7274,9 +7458,9 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
-      </c>
-      <c r="C16" s="14">
+        <v>243</v>
+      </c>
+      <c r="C16" s="13">
         <v>0.40277777777777773</v>
       </c>
     </row>
@@ -7285,9 +7469,9 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>237</v>
-      </c>
-      <c r="C17" s="14">
+        <v>234</v>
+      </c>
+      <c r="C17" s="13">
         <v>0.30416666666666664</v>
       </c>
     </row>
@@ -7296,9 +7480,9 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" s="14">
+        <v>251</v>
+      </c>
+      <c r="C18" s="13">
         <v>0.28611111111111115</v>
       </c>
     </row>
@@ -7307,40 +7491,40 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>253</v>
-      </c>
-      <c r="C19" s="14">
+        <v>250</v>
+      </c>
+      <c r="C19" s="13">
         <v>0.15069444444444444</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -7376,10 +7560,10 @@
       <c r="A1">
         <v>7</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="C1" s="17">
+      <c r="B1" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="16">
         <v>0.24097222222222223</v>
       </c>
     </row>
@@ -7387,10 +7571,10 @@
       <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="C2" s="17">
+      <c r="B2" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2" s="16">
         <v>0.31666666666666665</v>
       </c>
     </row>
@@ -7398,10 +7582,10 @@
       <c r="A3">
         <v>9</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="C3" s="17">
+      <c r="B3" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="16">
         <v>0.26527777777777778</v>
       </c>
     </row>
@@ -7409,10 +7593,10 @@
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="C4" s="17">
+      <c r="B4" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="16">
         <v>0.29305555555555557</v>
       </c>
     </row>
@@ -7420,10 +7604,10 @@
       <c r="A5">
         <v>11</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="C5" s="17">
+      <c r="B5" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" s="16">
         <v>0.26805555555555555</v>
       </c>
     </row>
@@ -7479,13 +7663,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1">
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added link for webinar
</commit_message>
<xml_diff>
--- a/data/training_videos.xlsx
+++ b/data/training_videos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24271C18-124E-434E-9E8D-2E3439F8AA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA378E6-2F27-0B46-BBB9-28E068378A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="426">
   <si>
     <t xml:space="preserve"> Arrangements  </t>
   </si>
@@ -1322,6 +1322,9 @@
   </si>
   <si>
     <t>How the instruments are laid out on the screen</t>
+  </si>
+  <si>
+    <t>https://youtu.be/vHaVhBcCGg0?si=b01u_o-XjEZZKYVQ</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1480,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1779,7 +1782,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1836,7 +1839,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1893,7 +1896,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1950,7 +1953,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2007,7 +2010,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3297,7 +3300,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisCol" showAll="0">
@@ -3405,19 +3408,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{486948C8-A13F-A545-90E9-87DFED66A023}" name="Table1" displayName="Table1" ref="A1:J116" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J116" xr:uid="{486948C8-A13F-A545-90E9-87DFED66A023}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Lighting"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A70:J116">
-    <sortCondition ref="A2:A116"/>
-    <sortCondition ref="B2:B116"/>
-    <sortCondition ref="C2:C116"/>
-    <sortCondition ref="D2:D116"/>
-  </sortState>
+  <autoFilter ref="A1:J116" xr:uid="{486948C8-A13F-A545-90E9-87DFED66A023}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{30A2E519-C016-EB48-A24E-8330D0AB56BC}" name="Topic1" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{BA07A1A3-1ECF-354E-8740-D7891A39DCB5}" name="Topic2" dataDxfId="8"/>
@@ -3933,8 +3924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="C101" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3983,7 +3974,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>84</v>
       </c>
@@ -4007,7 +3998,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>84</v>
       </c>
@@ -4031,7 +4022,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -4055,7 +4046,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>84</v>
       </c>
@@ -4079,7 +4070,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
@@ -4103,7 +4094,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>84</v>
       </c>
@@ -4127,7 +4118,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>84</v>
       </c>
@@ -4149,7 +4140,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>84</v>
       </c>
@@ -4178,7 +4169,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>84</v>
       </c>
@@ -4207,7 +4198,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
@@ -4236,7 +4227,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>84</v>
       </c>
@@ -4265,7 +4256,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>84</v>
       </c>
@@ -4294,7 +4285,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>84</v>
       </c>
@@ -4323,7 +4314,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>84</v>
       </c>
@@ -4347,7 +4338,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>84</v>
       </c>
@@ -4371,7 +4362,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>84</v>
       </c>
@@ -4398,7 +4389,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>84</v>
       </c>
@@ -4422,7 +4413,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
@@ -4446,7 +4437,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -4470,7 +4461,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>84</v>
       </c>
@@ -4493,7 +4484,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>84</v>
       </c>
@@ -4516,7 +4507,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>84</v>
       </c>
@@ -4539,7 +4530,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>84</v>
       </c>
@@ -4562,7 +4553,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>84</v>
       </c>
@@ -4585,7 +4576,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
@@ -4605,7 +4596,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>84</v>
       </c>
@@ -4626,7 +4617,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
@@ -4647,7 +4638,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>84</v>
       </c>
@@ -5500,7 +5491,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>206</v>
       </c>
@@ -5522,7 +5513,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>206</v>
       </c>
@@ -5549,7 +5540,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>206</v>
       </c>
@@ -5576,7 +5567,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>206</v>
       </c>
@@ -5606,7 +5597,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>206</v>
       </c>
@@ -5636,7 +5627,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>206</v>
       </c>
@@ -5666,7 +5657,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>83</v>
       </c>
@@ -5690,7 +5681,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>83</v>
       </c>
@@ -5714,7 +5705,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>83</v>
       </c>
@@ -5738,7 +5729,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>83</v>
       </c>
@@ -5762,7 +5753,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>83</v>
       </c>
@@ -5786,7 +5777,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>83</v>
       </c>
@@ -5815,7 +5806,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>83</v>
       </c>
@@ -5844,7 +5835,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>83</v>
       </c>
@@ -5876,7 +5867,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>83</v>
       </c>
@@ -5908,7 +5899,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>83</v>
       </c>
@@ -5937,7 +5928,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>83</v>
       </c>
@@ -5966,7 +5957,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>83</v>
       </c>
@@ -5998,7 +5989,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>83</v>
       </c>
@@ -6027,7 +6018,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
@@ -6059,7 +6050,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>83</v>
       </c>
@@ -6088,7 +6079,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>83</v>
       </c>
@@ -6117,7 +6108,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>83</v>
       </c>
@@ -6146,7 +6137,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>83</v>
       </c>
@@ -6175,7 +6166,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>83</v>
       </c>
@@ -6204,7 +6195,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
@@ -6233,7 +6224,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>83</v>
       </c>
@@ -6262,7 +6253,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>83</v>
       </c>
@@ -6291,7 +6282,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>79</v>
       </c>
@@ -6316,7 +6307,7 @@
       </c>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>79</v>
       </c>
@@ -6341,7 +6332,7 @@
       </c>
       <c r="J88" s="3"/>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>79</v>
       </c>
@@ -6366,7 +6357,7 @@
       </c>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>79</v>
       </c>
@@ -6388,7 +6379,7 @@
       </c>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>79</v>
       </c>
@@ -6407,7 +6398,7 @@
       </c>
       <c r="J91" s="3"/>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>79</v>
       </c>
@@ -6427,7 +6418,7 @@
       </c>
       <c r="J92" s="3"/>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>79</v>
       </c>
@@ -6448,7 +6439,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>79</v>
       </c>
@@ -6478,7 +6469,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>79</v>
       </c>
@@ -6508,7 +6499,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>79</v>
       </c>
@@ -6525,7 +6516,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>83</v>
       </c>
@@ -6552,7 +6543,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>83</v>
       </c>
@@ -6579,7 +6570,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>83</v>
       </c>
@@ -6604,7 +6595,7 @@
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>83</v>
       </c>
@@ -6629,7 +6620,7 @@
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>83</v>
       </c>
@@ -6654,7 +6645,7 @@
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>83</v>
       </c>
@@ -6679,7 +6670,7 @@
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>83</v>
       </c>
@@ -6704,7 +6695,7 @@
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>83</v>
       </c>
@@ -6729,7 +6720,7 @@
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>83</v>
       </c>
@@ -6754,7 +6745,7 @@
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>83</v>
       </c>
@@ -6779,7 +6770,7 @@
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>83</v>
       </c>
@@ -6804,7 +6795,7 @@
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>83</v>
       </c>
@@ -6829,7 +6820,7 @@
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>83</v>
       </c>
@@ -6854,7 +6845,7 @@
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>83</v>
       </c>
@@ -6879,7 +6870,7 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>83</v>
       </c>
@@ -6904,7 +6895,7 @@
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>83</v>
       </c>
@@ -6932,7 +6923,7 @@
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>83</v>
       </c>
@@ -6957,7 +6948,7 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
     </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>83</v>
       </c>
@@ -6982,7 +6973,7 @@
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
     </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>83</v>
       </c>
@@ -7007,7 +6998,7 @@
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>83</v>
       </c>
@@ -7026,7 +7017,9 @@
       <c r="F116" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="H116" s="3"/>
+      <c r="H116" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
     </row>
@@ -7067,11 +7060,12 @@
     <hyperlink ref="H71" r:id="rId27" xr:uid="{045D822F-D7EC-0843-BF87-B5E903B9062F}"/>
     <hyperlink ref="H100" r:id="rId28" location="219259" xr:uid="{AD0D256B-219F-2F46-BC7F-4D31F0C183BB}"/>
     <hyperlink ref="H101" r:id="rId29" location="218515" xr:uid="{807693E7-BD7A-3F4E-8C5A-771DA977A842}"/>
+    <hyperlink ref="H116" r:id="rId30" xr:uid="{90E05E38-9380-B544-977A-917E417A35EC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>